<commit_message>
sprint 14 cronjob work done
</commit_message>
<xml_diff>
--- a/media/reports/All_Output.xlsx
+++ b/media/reports/All_Output.xlsx
@@ -447,7 +447,7 @@
       </c>
       <c r="B1" t="inlineStr">
         <is>
-          <t xml:space="preserve"> </t>
+          <t>akhil</t>
         </is>
       </c>
     </row>
@@ -457,11 +457,7 @@
           <t>Organisation Name</t>
         </is>
       </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>rk</t>
-        </is>
-      </c>
+      <c r="B2" t="inlineStr"/>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
@@ -487,7 +483,7 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>2020-07-31</t>
+          <t>2020-09-04</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
sprint 15(for pagination and bug fixing)
</commit_message>
<xml_diff>
--- a/media/reports/All_Output.xlsx
+++ b/media/reports/All_Output.xlsx
@@ -44,7 +44,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -59,13 +59,21 @@
       <bottom style="thick"/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf borderId="1" fillId="2" fontId="1" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf borderId="2" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle builtinId="0" hidden="0" name="Normal" xfId="0"/>
@@ -431,7 +439,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E9"/>
+  <dimension ref="A1:E12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -457,7 +465,11 @@
           <t>Organisation Name</t>
         </is>
       </c>
-      <c r="B2" t="inlineStr"/>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>rk industries</t>
+        </is>
+      </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
@@ -483,7 +495,7 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>2020-09-04</t>
+          <t>2020-09-17</t>
         </is>
       </c>
     </row>
@@ -528,6 +540,67 @@
         <is>
           <t>Credit</t>
         </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="2" t="inlineStr">
+        <is>
+          <t>2020-09-10</t>
+        </is>
+      </c>
+      <c r="B10" s="2" t="inlineStr">
+        <is>
+          <t>test</t>
+        </is>
+      </c>
+      <c r="C10" s="2" t="inlineStr">
+        <is>
+          <t>Exp-1</t>
+        </is>
+      </c>
+      <c r="D10" s="2" t="inlineStr">
+        <is>
+          <t>EXPENSE</t>
+        </is>
+      </c>
+      <c r="E10" s="2" t="n">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="2" t="inlineStr">
+        <is>
+          <t>2020-09-10</t>
+        </is>
+      </c>
+      <c r="B11" s="2" t="inlineStr">
+        <is>
+          <t>test</t>
+        </is>
+      </c>
+      <c r="C11" s="2" t="inlineStr">
+        <is>
+          <t>Exp-2</t>
+        </is>
+      </c>
+      <c r="D11" s="2" t="inlineStr">
+        <is>
+          <t>EXPENSE</t>
+        </is>
+      </c>
+      <c r="E11" s="2" t="n">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="D12" s="1" t="inlineStr">
+        <is>
+          <t>TOTAL</t>
+        </is>
+      </c>
+      <c r="E12" s="1">
+        <f> SUM(E10:E11)</f>
+        <v/>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
sprint 16(debit note changes
</commit_message>
<xml_diff>
--- a/media/reports/All_Output.xlsx
+++ b/media/reports/All_Output.xlsx
@@ -439,7 +439,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E12"/>
+  <dimension ref="A1:E13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -495,7 +495,7 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>2020-09-17</t>
+          <t>2020-09-24</t>
         </is>
       </c>
     </row>
@@ -545,12 +545,12 @@
     <row r="10">
       <c r="A10" s="2" t="inlineStr">
         <is>
-          <t>2020-09-10</t>
+          <t>2020-09-22</t>
         </is>
       </c>
       <c r="B10" s="2" t="inlineStr">
         <is>
-          <t>test</t>
+          <t>expense</t>
         </is>
       </c>
       <c r="C10" s="2" t="inlineStr">
@@ -564,42 +564,67 @@
         </is>
       </c>
       <c r="E10" s="2" t="n">
-        <v>25</v>
+        <v>0</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="2" t="inlineStr">
         <is>
-          <t>2020-09-10</t>
+          <t>2020-09-22</t>
         </is>
       </c>
       <c r="B11" s="2" t="inlineStr">
         <is>
-          <t>test</t>
+          <t>TEST</t>
         </is>
       </c>
       <c r="C11" s="2" t="inlineStr">
         <is>
-          <t>Exp-2</t>
+          <t>CN-0001</t>
         </is>
       </c>
       <c r="D11" s="2" t="inlineStr">
         <is>
-          <t>EXPENSE</t>
+          <t>CREDITNOTE</t>
         </is>
       </c>
       <c r="E11" s="2" t="n">
-        <v>5</v>
+        <v>0</v>
       </c>
     </row>
     <row r="12">
-      <c r="D12" s="1" t="inlineStr">
+      <c r="A12" s="2" t="inlineStr">
+        <is>
+          <t>2020-09-23</t>
+        </is>
+      </c>
+      <c r="B12" s="2" t="inlineStr">
+        <is>
+          <t>TEST</t>
+        </is>
+      </c>
+      <c r="C12" s="2" t="inlineStr">
+        <is>
+          <t>CN-0002</t>
+        </is>
+      </c>
+      <c r="D12" s="2" t="inlineStr">
+        <is>
+          <t>CREDITNOTE</t>
+        </is>
+      </c>
+      <c r="E12" s="2" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="D13" s="1" t="inlineStr">
         <is>
           <t>TOTAL</t>
         </is>
       </c>
-      <c r="E12" s="1">
-        <f> SUM(E10:E11)</f>
+      <c r="E13" s="1">
+        <f> SUM(E10:E12)</f>
         <v/>
       </c>
     </row>

</xml_diff>

<commit_message>
sprint 16(changes suggested by nikhil sir)
</commit_message>
<xml_diff>
--- a/media/reports/All_Output.xlsx
+++ b/media/reports/All_Output.xlsx
@@ -439,7 +439,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E13"/>
+  <dimension ref="A1:E14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -495,7 +495,7 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>2020-09-24</t>
+          <t>2020-10-02</t>
         </is>
       </c>
     </row>
@@ -573,16 +573,8 @@
           <t>2020-09-22</t>
         </is>
       </c>
-      <c r="B11" s="2" t="inlineStr">
-        <is>
-          <t>TEST</t>
-        </is>
-      </c>
-      <c r="C11" s="2" t="inlineStr">
-        <is>
-          <t>CN-0001</t>
-        </is>
-      </c>
+      <c r="B11" s="2" t="n"/>
+      <c r="C11" s="2" t="n"/>
       <c r="D11" s="2" t="inlineStr">
         <is>
           <t>CREDITNOTE</t>
@@ -598,16 +590,8 @@
           <t>2020-09-23</t>
         </is>
       </c>
-      <c r="B12" s="2" t="inlineStr">
-        <is>
-          <t>TEST</t>
-        </is>
-      </c>
-      <c r="C12" s="2" t="inlineStr">
-        <is>
-          <t>CN-0002</t>
-        </is>
-      </c>
+      <c r="B12" s="2" t="n"/>
+      <c r="C12" s="2" t="n"/>
       <c r="D12" s="2" t="inlineStr">
         <is>
           <t>CREDITNOTE</t>
@@ -618,13 +602,30 @@
       </c>
     </row>
     <row r="13">
-      <c r="D13" s="1" t="inlineStr">
+      <c r="A13" s="2" t="inlineStr">
+        <is>
+          <t>2020-09-24</t>
+        </is>
+      </c>
+      <c r="B13" s="2" t="n"/>
+      <c r="C13" s="2" t="n"/>
+      <c r="D13" s="2" t="inlineStr">
+        <is>
+          <t>CREDITNOTE</t>
+        </is>
+      </c>
+      <c r="E13" s="2" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="D14" s="1" t="inlineStr">
         <is>
           <t>TOTAL</t>
         </is>
       </c>
-      <c r="E13" s="1">
-        <f> SUM(E10:E12)</f>
+      <c r="E14" s="1">
+        <f> SUM(E10:E13)</f>
         <v/>
       </c>
     </row>

</xml_diff>